<commit_message>
Added dependencies for different proms but same prof
</commit_message>
<xml_diff>
--- a/professors.xlsx
+++ b/professors.xlsx
@@ -13,17 +13,17 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1619815321" val="982" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1619815321" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1619815321" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1619815321"/>
+      <pm:revision xmlns:pm="smNativeData" day="1619953611" val="982" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1619953611" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1619953611" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1619953611"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>Name</t>
   </si>
@@ -44,9 +44,6 @@
   </si>
   <si>
     <t>Merken</t>
-  </si>
-  <si>
-    <t>1-&gt;4</t>
   </si>
   <si>
     <t>no</t>
@@ -103,7 +100,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1619815321" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1619953611" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -118,7 +115,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1619815321" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1619953611" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -140,7 +137,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1619815321" type="1" fgLvl="100" fgClr="00000000" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1619953611" type="1" fgLvl="100" fgClr="00000000" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -151,7 +148,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1619815321" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1619953611" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -173,7 +170,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1619815321"/>
+          <pm:border xmlns:pm="smNativeData" id="1619953611"/>
         </ext>
       </extLst>
     </border>
@@ -192,7 +189,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1619815321"/>
+          <pm:border xmlns:pm="smNativeData" id="1619953611"/>
         </ext>
       </extLst>
     </border>
@@ -211,7 +208,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1619815321"/>
+          <pm:border xmlns:pm="smNativeData" id="1619953611"/>
         </ext>
       </extLst>
     </border>
@@ -233,7 +230,7 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1619815321" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1619953611" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
     </ext>
@@ -515,7 +512,7 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.660714" defaultRowHeight="15.40"/>
@@ -553,11 +550,9 @@
       <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="B2" s="1"/>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" s="3" t="n">
         <v>44346</v>
@@ -566,7 +561,7 @@
         <v>44367</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -574,96 +569,96 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" t="n">
         <v>3</v>
       </c>
       <c r="F5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" t="n">
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="36" spans="1:1">
@@ -681,7 +676,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1619815321" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1619953611" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -690,8 +685,8 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1619815321" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1619815321" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1619953611" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1619953611" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
@@ -700,7 +695,7 @@
   </tableParts>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1619815321" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1619953611" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
Cleaning and explanations in Dummy example
</commit_message>
<xml_diff>
--- a/professors.xlsx
+++ b/professors.xlsx
@@ -1,27 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileSharing readOnlyRecommended="0" userName="sputnik"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simplex\Documents\ERM\1Ma\sem2\DS425_E\ProjetHoraireExam\ExamTimetable\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3D1009A-B858-48C8-9D38-45FF62AF4077}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" xWindow="240" yWindow="60" windowWidth="23260" windowHeight="12578" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Professors" sheetId="1" r:id="rId1"/>
+    <sheet name="Professors" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1619953611" val="982" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1619953611" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1619953611" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1619953611"/>
+      <pm:revision xmlns:pm="smNativeData" day="1619965088" val="982" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1619965088" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1619965088" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1619965088"/>
     </ext>
   </extLst>
 </workbook>
@@ -48,10 +43,13 @@
     <t>is weekend ok? (yes/no)</t>
   </si>
   <si>
+    <t>no</t>
+  </si>
+  <si>
     <t>Merken</t>
   </si>
   <si>
-    <t>no</t>
+    <t>yes</t>
   </si>
   <si>
     <t>Van Utterbeek</t>
@@ -64,9 +62,6 @@
   </si>
   <si>
     <t>Coghe</t>
-  </si>
-  <si>
-    <t>yes</t>
   </si>
   <si>
     <t>Galant</t>
@@ -84,66 +79,159 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="h:mm"/>
-    <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="10">
+    <numFmt numFmtId="5" formatCode="#,##0\ &quot;$&quot;;\-#,##0\ &quot;$&quot;"/>
+    <numFmt numFmtId="6" formatCode="#,##0\ &quot;$&quot;;[Red]\-#,##0\ &quot;$&quot;"/>
+    <numFmt numFmtId="7" formatCode="#,##0.00\ &quot;$&quot;;\-#,##0.00\ &quot;$&quot;"/>
+    <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;$&quot;;[Red]\-#,##0.00\ &quot;$&quot;"/>
+    <numFmt numFmtId="42" formatCode="_-* #,##0\ &quot;$&quot;_-;\-* #,##0\ &quot;$&quot;_-;_-* &quot;-&quot;\ &quot;$&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0\ _$_-;\-* #,##0\ _$_-;_-* &quot;-&quot;\ _$_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;$&quot;_-;\-* #,##0.00\ &quot;$&quot;_-;_-* &quot;-&quot;??\ &quot;$&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _$_-;\-* #,##0.00\ _$_-;_-* &quot;-&quot;??\ _$_-;_-@_-"/>
+    <numFmt numFmtId="20" formatCode="h:mm"/>
+    <numFmt numFmtId="14" formatCode="M/D/YYYY"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1619965088" ulstyle="none" kern="1">
+            <pm:latin face="Calibri" sz="220" lang="default"/>
+            <pm:cs face="Basic Roman" sz="220" lang="default"/>
+            <pm:ea face="Basic Roman" sz="220" lang="default"/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
+    </font>
+    <font>
+      <name val="Basic Sans"/>
+      <family val="1"/>
+      <color rgb="FF000000"/>
+      <sz val="10"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1619965088" ulstyle="none" kern="1">
+            <pm:latin face="Basic Sans" sz="200" lang="default"/>
+            <pm:cs face="Basic Roman" sz="200" lang="default"/>
+            <pm:ea face="Basic Roman" sz="200" lang="default"/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1619965088" type="1" fgLvl="100" fgClr="00000000" bgLvl="100" bgClr="00000000"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1619965088" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1619965088"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1619965088"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1619965088"/>
+        </ext>
+      </extLst>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
-      <protection hidden="1"/>
+      <protection locked="1" hidden="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-  </dxfs>
   <tableStyles count="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1619953611" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1619965088" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
     </ext>
@@ -152,15 +240,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:F10" totalsRowShown="0">
-  <autoFilter ref="A1:F10" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table2" displayName="Table2" ref="A1:F10" totalsRowShown="0">
+  <autoFilter ref="A1:F10"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" totalsRowLabel="Total"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Unavailability"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Parallel exams"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="start date"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="final date"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="is weekend ok? (yes/no)" totalsRowFunction="sum" dataDxfId="0"/>
+    <tableColumn id="1" name="Name" totalsRowLabel="Total"/>
+    <tableColumn id="2" name="Unavailability"/>
+    <tableColumn id="3" name="Parallel exams"/>
+    <tableColumn id="4" name="start date"/>
+    <tableColumn id="5" name="final date"/>
+    <tableColumn id="6" name="is weekend ok? (yes/no)" totalsRowFunction="sum"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -421,27 +509,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" view="normal" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.660714" defaultRowHeight="15.40"/>
   <cols>
-    <col min="1" max="1" width="15.77734375" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" customWidth="1"/>
-    <col min="3" max="3" width="18.109375" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" customWidth="1"/>
-    <col min="6" max="6" width="25" style="4" customWidth="1"/>
-    <col min="7" max="7" width="25" customWidth="1"/>
-    <col min="8" max="8" width="13.44140625" customWidth="1"/>
-    <col min="9" max="9" width="14.33203125" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="3.5546875" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="15.776786" customWidth="1"/>
+    <col min="2" max="2" width="16.437500" customWidth="1"/>
+    <col min="3" max="3" width="18.107143" customWidth="1"/>
+    <col min="4" max="4" width="14.330357" customWidth="1"/>
+    <col min="6" max="6" width="25.000000" customWidth="1" style="4"/>
+    <col min="7" max="7" width="25.000000" customWidth="1"/>
+    <col min="8" max="8" width="13.437500" customWidth="1"/>
+    <col min="9" max="9" width="14.330357" hidden="1" customWidth="1">
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:columnDef xmlns:pm="smNativeData" id="1619965088" min="9" max="9" hidden="1" collapsedDB="0" collapsedOL="0"/>
+        </ext>
+      </extLst>
+    </col>
+    <col min="10" max="10" width="3.553571" hidden="1" customWidth="1">
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:columnDef xmlns:pm="smNativeData" id="1619965088" min="10" max="10" hidden="1" collapsedDB="0" collapsedOL="0"/>
+        </ext>
+      </extLst>
+    </col>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -461,178 +561,199 @@
         <v>5</v>
       </c>
       <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3" t="n">
+        <v>44346</v>
+      </c>
+      <c r="E2" s="3" t="n">
+        <v>44367</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="1"/>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2" s="3">
-        <v>44346</v>
-      </c>
-      <c r="E2" s="3">
-        <v>44367</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>7</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" t="n">
+        <v>2</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" t="n">
+        <v>2</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" t="s">
         <v>12</v>
       </c>
-      <c r="J2" t="s">
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" t="n">
+        <v>2</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5">
-        <v>3</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>12</v>
       </c>
       <c r="J6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="1"/>
-      <c r="C7">
+      <c r="C7" t="n">
         <v>1</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="1"/>
-      <c r="C8">
+      <c r="C8" t="n">
         <v>2</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>15</v>
       </c>
-      <c r="C9">
+      <c r="C9" t="n">
         <v>1</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>16</v>
       </c>
-      <c r="C10">
+      <c r="C10" t="n">
         <v>2</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
       <c r="A36" s="2"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1">
       <c r="A37" s="2"/>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select option" sqref="F2:F1048576" xr:uid="{3D964693-3981-4BA8-BEC6-C1A32B234431}">
+    <dataValidation sqref="A1" type="none" operator="between" errorStyle="stop" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select name" view="0">
+      <formula1/>
+      <formula2/>
+    </dataValidation>
+    <dataValidation sqref="F1" type="none" operator="between" errorStyle="stop" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select option" view="0">
+      <formula1/>
+      <formula2/>
+    </dataValidation>
+    <dataValidation sqref="A2:A1048576" type="list" operator="between" errorStyle="stop" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select name" view="0">
+      <formula1>$J$1:$J$9</formula1>
+    </dataValidation>
+    <dataValidation sqref="F2:F1048576" type="list" operator="between" errorStyle="stop" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select option" view="0">
       <formula1>$I$1:$I$2</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select name" sqref="A2:A1048576" xr:uid="{71969A32-4D22-458E-A219-30BDB8764336}">
-      <formula1>$J$1:$J$9</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select option" sqref="F1" xr:uid="{435AA1DA-E722-4331-ACB3-5F63232F7EFF}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select name" sqref="A1" xr:uid="{6CB3D6C9-7C66-4CF1-9181-DC20DE04B5F8}"/>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup fitToWidth="0" orientation="portrait" r:id="rId1"/>
+  <printOptions>
+    <extLst>
+      <ext uri="smNativeData">
+        <pm:pageFlags xmlns:pm="smNativeData" id="1619965088" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+      </ext>
+    </extLst>
+  </printOptions>
+  <pageMargins left="0.700000" right="0.700000" top="0.750000" bottom="0.750000" header="0.300000" footer="0.300000"/>
+  <pageSetup paperSize="1" fitToWidth="0" fitToHeight="1"/>
+  <headerFooter>
+    <extLst>
+      <ext uri="smNativeData">
+        <pm:header xmlns:pm="smNativeData" id="1619965088" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1619965088" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+      </ext>
+    </extLst>
+  </headerFooter>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1619953611" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1619965088" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>